<commit_message>
register/shadow, register/external, register/accessibilityをregister/type, register/types/indirect, register/types/externalで置換(#8)
</commit_message>
<xml_diff>
--- a/sample/sample.xlsx
+++ b/sample/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>block name</t>
   </si>
@@ -143,12 +143,6 @@
   </si>
   <si>
     <t>bit_field_4_1</t>
-  </si>
-  <si>
-    <t>shadow index</t>
-  </si>
-  <si>
-    <t>shdow index</t>
   </si>
   <si>
     <t>0x20</t>
@@ -170,7 +164,111 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>bit_field_2_1:1, bit_field_0_0, bit_field_0_1</t>
+    <t>0x80-0xFF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>[8]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bit_field_6_0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>w0c</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bit_field_6_1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>w1c</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>register_6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>0x28</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>register_7</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>[8]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bit_field_7_0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>w0s</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bit_field_7_1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>w1s</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>register_8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>[31:16]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>rwl</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>[15:0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>bit_field_8_1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>rwe</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>register_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_8_0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>0x2C</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>indirect: bit_field_2_1:1, bit_field_0_0, bit_field_0_1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -178,112 +276,8 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0x80-0xFF</t>
+    <t>type</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x24</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>[8]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>bit_field_6_0</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>w0c</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>[0]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>bit_field_6_1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>w1c</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>register_6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>0x28</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>register_7</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>[8]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>bit_field_7_0</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>w0s</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>[0]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>bit_field_7_1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>w1s</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>register_8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>[31:16]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>rwl</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>[15:0]</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>bit_field_8_1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>rwe</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>register_9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_8_0</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>0x2C</t>
-    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -546,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -567,7 +561,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -910,7 +903,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K21"/>
+  <dimension ref="B1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -918,10 +911,10 @@
   <cols>
     <col min="2" max="4" width="15.75" customWidth="1"/>
     <col min="5" max="5" width="40.75" customWidth="1"/>
-    <col min="6" max="11" width="15.75" customWidth="1"/>
+    <col min="6" max="10" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -929,7 +922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>27</v>
       </c>
@@ -937,8 +930,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
@@ -949,28 +942,25 @@
         <v>35</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
@@ -979,42 +969,40 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="G5" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1023,22 +1011,21 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1047,40 +1034,38 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I8" s="1"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1089,20 +1074,19 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G10" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I10" s="1"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1113,242 +1097,231 @@
         <v>38</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G11" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I11" s="1"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="E13" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="H13" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I13" s="1"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="G14" s="13" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="H14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="19">
+        <v>0</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="19">
+        <v>0</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B17" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="19">
+        <v>0</v>
+      </c>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="19">
+        <v>0</v>
+      </c>
+      <c r="J18" s="21"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B19" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" s="19">
+        <v>0</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B15" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" s="20">
-        <v>0</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="J16" s="20">
-        <v>0</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B17" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="J17" s="20">
-        <v>0</v>
-      </c>
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="J18" s="20">
-        <v>0</v>
-      </c>
-      <c r="K18" s="22"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B19" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21" t="s">
+      <c r="C21" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="J19" s="20">
-        <v>0</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="I20" s="21" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J20" s="20">
-        <v>0</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="18" t="s">
-        <v>52</v>
-      </c>
+      <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
+      <c r="J21" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1358,16 +1331,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K9"/>
+  <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="11" width="15.75" customWidth="1"/>
+    <col min="2" max="10" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1383,8 +1356,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1395,28 +1368,25 @@
         <v>35</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1425,40 +1395,38 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="G5" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1467,22 +1435,21 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1491,38 +1458,36 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="1"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="2:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="G9" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6"/>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>